<commit_message>
Test of xlsx DSW1
</commit_message>
<xml_diff>
--- a/Scripts_til_Cybernetvaerk/Adressing table.xlsx
+++ b/Scripts_til_Cybernetvaerk/Adressing table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Site2Git\Scripts_til_Cybernetvaerk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Site2Git\Scripts_til_Cybernetvaerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Site 2</t>
   </si>
@@ -40,13 +40,100 @@
   </si>
   <si>
     <t>Som er meget bedre end de andre sites</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>Subnet Mask</t>
+  </si>
+  <si>
+    <t>Default Gateway</t>
+  </si>
+  <si>
+    <t>DSW1</t>
+  </si>
+  <si>
+    <t>Gi1/0/1</t>
+  </si>
+  <si>
+    <t>VLAN4 10.1.4.6, 2026:2::2/64</t>
+  </si>
+  <si>
+    <t>Gi1/0/23</t>
+  </si>
+  <si>
+    <t>VLAN1 10.2.4.13, 2026:3::1/64</t>
+  </si>
+  <si>
+    <t>Loopback1</t>
+  </si>
+  <si>
+    <t>11.11.11.11/32</t>
+  </si>
+  <si>
+    <t>FEC0:11::1/64</t>
+  </si>
+  <si>
+    <t>VLAN1</t>
+  </si>
+  <si>
+    <t>10.2.4.13, 2026:3::1/64</t>
+  </si>
+  <si>
+    <t>VLAN4</t>
+  </si>
+  <si>
+    <t>10.1.4.6, 2026:2::2/64</t>
+  </si>
+  <si>
+    <t>VLAN10</t>
+  </si>
+  <si>
+    <t>10.2.1.1, 2026:10::1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255.255.255.0, /64 </t>
+  </si>
+  <si>
+    <t>VLAN20</t>
+  </si>
+  <si>
+    <t>10.2.2.1, 2026:20::1</t>
+  </si>
+  <si>
+    <t>255.255.255.0, /64</t>
+  </si>
+  <si>
+    <t>VLAN150</t>
+  </si>
+  <si>
+    <t>10.2.3.1</t>
+  </si>
+  <si>
+    <t>VLAN200</t>
+  </si>
+  <si>
+    <t>192.168.1.129</t>
+  </si>
+  <si>
+    <t>VLAN250</t>
+  </si>
+  <si>
+    <t>10.2.3.129</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +141,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE5F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -71,12 +177,127 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -410,13 +631,186 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5">
+        <v>255255255252</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5">
+        <v>255255255252</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5">
+        <v>255255255252</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5">
+        <v>255255255252</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5">
+        <v>255255255128</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5">
+        <v>255255255224</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5">
+        <v>255255255224</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Nu med addresing table template
</commit_message>
<xml_diff>
--- a/Scripts_til_Cybernetvaerk/Adressing table.xlsx
+++ b/Scripts_til_Cybernetvaerk/Adressing table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Site2Git\Scripts_til_Cybernetvaerk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Administrator\Docs\Site2Git\Scripts_til_Cybernetvaerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Site 2</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>10.2.3.129</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Subnetmask</t>
+  </si>
+  <si>
+    <t>Default gateway</t>
   </si>
 </sst>
 </file>
@@ -155,7 +164,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,8 +177,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -262,11 +301,218 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -298,6 +544,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,12 +886,128 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="5" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -633,7 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
@@ -691,7 +1074,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>14</v>
@@ -702,7 +1085,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="10"/>
       <c r="C5" s="4" t="s">

</xml_diff>

<commit_message>
ASW1 Addressing opdateret for LAB 4.3.8
</commit_message>
<xml_diff>
--- a/Scripts_til_Cybernetvaerk/Adressing table.xlsx
+++ b/Scripts_til_Cybernetvaerk/Adressing table.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Site 2</t>
   </si>
@@ -136,6 +136,57 @@
   </si>
   <si>
     <t>Default gateway</t>
+  </si>
+  <si>
+    <t>Gi1/0/1-2(23)</t>
+  </si>
+  <si>
+    <t>VLAN 250 Access Mode</t>
+  </si>
+  <si>
+    <t>VLAN 10</t>
+  </si>
+  <si>
+    <t>VLAN 20</t>
+  </si>
+  <si>
+    <t>VLAN 150</t>
+  </si>
+  <si>
+    <t>VLAN 200</t>
+  </si>
+  <si>
+    <t>VLAN 250</t>
+  </si>
+  <si>
+    <t>192.168.1.132</t>
+  </si>
+  <si>
+    <t>192.168.1.130</t>
+  </si>
+  <si>
+    <t>ASW2</t>
+  </si>
+  <si>
+    <t>VLAN 20 Access Mode</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Gi1/0/24</t>
+  </si>
+  <si>
+    <t>Gi1/0/19</t>
+  </si>
+  <si>
+    <t>TRUNK Native 99</t>
+  </si>
+  <si>
+    <t>Gi1/0/21</t>
+  </si>
+  <si>
+    <t>Access20 Voice150</t>
   </si>
 </sst>
 </file>
@@ -512,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -565,6 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,14 +941,15 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="5" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -917,79 +970,125 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
+      <c r="A2" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="B2" s="16"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
+      <c r="E2" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
+      <c r="B3" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="D3" s="21"/>
       <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
+      <c r="B4" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>50</v>
+      </c>
       <c r="D4" s="25"/>
       <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="27"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
+      <c r="B5" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>50</v>
+      </c>
       <c r="D5" s="21"/>
       <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
+      <c r="B7" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>37</v>
+      </c>
       <c r="D7" s="21"/>
       <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
+      <c r="B8" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>47</v>
+      </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
+      <c r="B9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>47</v>
+      </c>
       <c r="D9" s="21"/>
       <c r="E9" s="22"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
+      <c r="B10" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="32">
+        <v>255255255224</v>
+      </c>
       <c r="E11" s="22"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
+      <c r="B12" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>47</v>
+      </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
     </row>
@@ -1017,7 +1116,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DSW2 update - incomplete. encaptulation still fucking
</commit_message>
<xml_diff>
--- a/Scripts_til_Cybernetvaerk/Adressing table.xlsx
+++ b/Scripts_til_Cybernetvaerk/Adressing table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Site2Git\Scripts_til_Cybernetvaerk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Site2Git\Scripts_til_Cybernetvaerk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>Site 2</t>
   </si>
@@ -127,6 +127,90 @@
   </si>
   <si>
     <t>10.2.3.129</t>
+  </si>
+  <si>
+    <t>10.1.4.10</t>
+  </si>
+  <si>
+    <t>IPv4</t>
+  </si>
+  <si>
+    <t>SubnetMask</t>
+  </si>
+  <si>
+    <t>IPv6</t>
+  </si>
+  <si>
+    <t>VLAN5</t>
+  </si>
+  <si>
+    <t>10.2.4.14</t>
+  </si>
+  <si>
+    <t>2026:3::2/64</t>
+  </si>
+  <si>
+    <t>Har "ekstra" IPv6 2026:3::1</t>
+  </si>
+  <si>
+    <t>Loopback2</t>
+  </si>
+  <si>
+    <t>22.22.22.22</t>
+  </si>
+  <si>
+    <t>Tilføj IPv6</t>
+  </si>
+  <si>
+    <t>Tilføj IPv6?</t>
+  </si>
+  <si>
+    <t>10.2.1.2</t>
+  </si>
+  <si>
+    <t>10.2.2.2</t>
+  </si>
+  <si>
+    <t>10.2.3.2</t>
+  </si>
+  <si>
+    <t>192.168.1.130</t>
+  </si>
+  <si>
+    <t>10.2.3.130</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>2026:10::2</t>
+  </si>
+  <si>
+    <t>2026:20::2</t>
+  </si>
+  <si>
+    <t>No IPv6</t>
+  </si>
+  <si>
+    <t>2026:4::2/64</t>
+  </si>
+  <si>
+    <t>Gi1/0/19</t>
+  </si>
+  <si>
+    <t>Trunk</t>
+  </si>
+  <si>
+    <t>10,20,150,200,250</t>
+  </si>
+  <si>
+    <t>10,20,150,200,251</t>
+  </si>
+  <si>
+    <t>Gi1/0/21</t>
+  </si>
+  <si>
+    <t>FEC0:22::2/64</t>
   </si>
 </sst>
 </file>
@@ -266,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -298,6 +382,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
@@ -691,7 +776,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>14</v>
@@ -702,7 +787,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="10"/>
       <c r="C5" s="4" t="s">
@@ -816,14 +901,213 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="11">
+        <v>255255255252</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="11">
+        <v>255255255252</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="11">
+        <v>255255255252</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="11">
+        <v>255255255252</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="11">
+        <v>255255255252</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="11">
+        <v>255255255128</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="11">
+        <v>255255255224</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="11">
+        <v>255255255128</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>